<commit_message>
Updated: SchemaDefinition; Added: SchemaDiagram (png/pdf)
</commit_message>
<xml_diff>
--- a/SchemaDefinition.xlsx
+++ b/SchemaDefinition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7160"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="80">
   <si>
     <t>Entity</t>
   </si>
@@ -74,9 +74,6 @@
     <t>PK</t>
   </si>
   <si>
-    <t>day</t>
-  </si>
-  <si>
     <t>char</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>[1,20]</t>
   </si>
   <si>
-    <t>room_no</t>
-  </si>
-  <si>
     <t>capacity</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>Department</t>
   </si>
   <si>
-    <t>dept_name</t>
-  </si>
-  <si>
     <t>{CSE,MTH,CHM,BIO,HUM,ECE,SWE,PSY}</t>
   </si>
   <si>
@@ -152,9 +143,6 @@
     <t>FK</t>
   </si>
   <si>
-    <t>tot_cred</t>
-  </si>
-  <si>
     <t>[0,130]</t>
   </si>
   <si>
@@ -173,9 +161,6 @@
     <t>course_id</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
     <t>credits</t>
   </si>
   <si>
@@ -188,12 +173,6 @@
     <t>SF*2500*0.9</t>
   </si>
   <si>
-    <t>s_id</t>
-  </si>
-  <si>
-    <t>i_id</t>
-  </si>
-  <si>
     <t>Prereq</t>
   </si>
   <si>
@@ -209,9 +188,6 @@
     <t>SF*100*2.5*3</t>
   </si>
   <si>
-    <t>sec_id</t>
-  </si>
-  <si>
     <t>semester</t>
   </si>
   <si>
@@ -237,6 +213,57 @@
   </si>
   <si>
     <t>[A,F]</t>
+  </si>
+  <si>
+    <t>[30000,150000]</t>
+  </si>
+  <si>
+    <t>[2000,2016]</t>
+  </si>
+  <si>
+    <t>[1,10]</t>
+  </si>
+  <si>
+    <t>{MWF,TR}</t>
+  </si>
+  <si>
+    <t>[1,30]</t>
+  </si>
+  <si>
+    <t>INCREMENT(1,1) &lt;= 17</t>
+  </si>
+  <si>
+    <t>INCREMENT(1,1) &lt;= SF*2500</t>
+  </si>
+  <si>
+    <t>INCREMENT(1,1) &lt;= SF*100</t>
+  </si>
+  <si>
+    <t>SF*100</t>
+  </si>
+  <si>
+    <t>INCREMENT(1,1) &lt;= SF*100*2.5</t>
+  </si>
+  <si>
+    <t>student_id</t>
+  </si>
+  <si>
+    <t>instructor_id</t>
+  </si>
+  <si>
+    <t>room_number</t>
+  </si>
+  <si>
+    <t>department_name</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>section_number</t>
+  </si>
+  <si>
+    <t>days</t>
   </si>
 </sst>
 </file>
@@ -579,24 +606,25 @@
   <dimension ref="A1:K67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7265625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,13 +659,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -652,9 +680,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -666,7 +694,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>15</v>
@@ -676,66 +704,69 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
+        <v>36</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2">
@@ -745,9 +776,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -759,7 +790,7 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>15</v>
@@ -769,15 +800,21 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>15</v>
@@ -787,9 +824,9 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
@@ -801,22 +838,22 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H14" s="2">
         <v>8</v>
@@ -829,12 +866,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="2">
         <v>3</v>
@@ -843,7 +880,7 @@
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>15</v>
@@ -853,9 +890,9 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -867,16 +904,16 @@
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -888,25 +925,25 @@
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2">
@@ -916,12 +953,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>13</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>69</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>15</v>
@@ -931,12 +974,12 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -945,19 +988,19 @@
         <v>32</v>
       </c>
       <c r="F21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="2">
         <v>3</v>
@@ -966,21 +1009,21 @@
         <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
@@ -992,24 +1035,26 @@
         <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2">
         <v>2</v>
@@ -1018,27 +1063,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
         <v>13</v>
       </c>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>70</v>
+      </c>
       <c r="G26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
@@ -1047,19 +1097,19 @@
         <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" s="2">
         <v>3</v>
@@ -1068,42 +1118,51 @@
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
         <v>13</v>
+      </c>
+      <c r="D29" s="2">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2">
+        <v>6</v>
+      </c>
+      <c r="F29" t="s">
+        <v>63</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2">
@@ -1113,12 +1172,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
         <v>13</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>72</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>15</v>
@@ -1128,12 +1193,12 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D33" s="2">
         <v>1</v>
@@ -1142,19 +1207,19 @@
         <v>32</v>
       </c>
       <c r="F33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D34" s="2">
         <v>3</v>
@@ -1163,21 +1228,21 @@
         <v>3</v>
       </c>
       <c r="F34" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
         <v>13</v>
@@ -1189,25 +1254,25 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2">
@@ -1217,52 +1282,58 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
         <v>13</v>
       </c>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
       <c r="G39" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2">
@@ -1272,42 +1343,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
+      <c r="I42" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
+      <c r="I43" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-    </row>
-    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2">
@@ -1317,41 +1398,55 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C46" t="s">
         <v>13</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>61</v>
+        <v>77</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>65</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D48" s="2">
         <v>4</v>
@@ -1360,7 +1455,7 @@
         <v>6</v>
       </c>
       <c r="F48" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>15</v>
@@ -1370,8 +1465,20 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="2">
+        <v>4</v>
+      </c>
+      <c r="E49" s="2">
+        <v>4</v>
+      </c>
+      <c r="F49" t="s">
         <v>64</v>
       </c>
       <c r="G49" s="2" t="s">
@@ -1382,9 +1489,9 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C50" t="s">
         <v>13</v>
@@ -1396,21 +1503,21 @@
         <v>2</v>
       </c>
       <c r="F50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="C51" t="s">
         <v>13</v>
@@ -1418,17 +1525,23 @@
       <c r="D51" s="2">
         <v>1</v>
       </c>
+      <c r="E51" s="2">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>67</v>
+      </c>
       <c r="G51" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>12</v>
       </c>
@@ -1445,7 +1558,7 @@
         <v>14</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2" t="s">
@@ -1454,18 +1567,18 @@
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2">
@@ -1475,60 +1588,78 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="C55" t="s">
         <v>13</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C56" t="s">
         <v>13</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
-        <v>61</v>
+        <v>78</v>
+      </c>
+      <c r="C57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2">
+        <v>2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>65</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D58" s="2">
         <v>4</v>
@@ -1537,20 +1668,32 @@
         <v>6</v>
       </c>
       <c r="F58" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="2">
+        <v>4</v>
+      </c>
+      <c r="E59" s="2">
+        <v>4</v>
+      </c>
+      <c r="F59" t="s">
         <v>64</v>
       </c>
       <c r="G59" s="2" t="s">
@@ -1558,23 +1701,23 @@
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="2">
@@ -1584,60 +1727,78 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="C62" t="s">
         <v>13</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C63" t="s">
         <v>13</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
-        <v>61</v>
+        <v>78</v>
+      </c>
+      <c r="C64" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2">
+        <v>2</v>
+      </c>
+      <c r="F64" t="s">
+        <v>65</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D65" s="2">
         <v>4</v>
@@ -1646,20 +1807,32 @@
         <v>6</v>
       </c>
       <c r="F65" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
+        <v>56</v>
+      </c>
+      <c r="C66" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="2">
+        <v>4</v>
+      </c>
+      <c r="E66" s="2">
+        <v>4</v>
+      </c>
+      <c r="F66" t="s">
         <v>64</v>
       </c>
       <c r="G66" s="2" t="s">
@@ -1667,17 +1840,17 @@
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D67" s="2">
         <v>1</v>
@@ -1686,7 +1859,7 @@
         <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>

</xml_diff>